<commit_message>
Product backlog + handleiding
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\Documents\HR\Project 4\Project-4-Developing-a-cross-platform-application-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\Documents\HR\Project 4\Developing-a-cross-platform-application-\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6370" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>- make a diagram with astah (de eerste versie)</t>
   </si>
   <si>
     <t>Als developer wil ik comments bij alle code hebben staan, zodat ik snel de code kan begrijpen.</t>
@@ -199,6 +196,15 @@
   </si>
   <si>
     <t>Als user wil ik een bal die van de horizontale kanten kaatst, zodat ik het spel kan spelen.</t>
+  </si>
+  <si>
+    <t>Maak een diagram met astah (de eerste versie)</t>
+  </si>
+  <si>
+    <t>Update diagram in astah.</t>
+  </si>
+  <si>
+    <t>Het diagram is up to date met de het design.</t>
   </si>
 </sst>
 </file>
@@ -404,9 +410,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -458,16 +461,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -487,6 +480,19 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -816,50 +822,50 @@
   <dimension ref="A1:F997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="24" customWidth="1"/>
-    <col min="2" max="2" width="102.54296875" style="24" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="24" customWidth="1"/>
-    <col min="5" max="13" width="11.453125" style="24" customWidth="1"/>
-    <col min="14" max="14" width="8.54296875" style="24" customWidth="1"/>
-    <col min="15" max="16384" width="17.453125" style="24"/>
+    <col min="1" max="1" width="5" style="23" customWidth="1"/>
+    <col min="2" max="2" width="102.54296875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" style="23" customWidth="1"/>
+    <col min="5" max="13" width="11.453125" style="23" customWidth="1"/>
+    <col min="14" max="14" width="8.54296875" style="23" customWidth="1"/>
+    <col min="15" max="16384" width="17.453125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -867,8 +873,8 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>17</v>
+      <c r="B3" s="28" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -881,61 +887,63 @@
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="4"/>
+      <c r="D4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="E5" s="16"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="17" t="s">
-        <v>39</v>
+      <c r="E7" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -943,10 +951,10 @@
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="4"/>
@@ -957,10 +965,10 @@
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="4"/>
@@ -971,11 +979,11 @@
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>23</v>
+      <c r="B10" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -985,11 +993,11 @@
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -999,15 +1007,15 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>23</v>
+      <c r="B12" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="17" t="s">
-        <v>39</v>
+      <c r="E12" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="F12" s="4"/>
     </row>
@@ -1015,29 +1023,29 @@
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>23</v>
+      <c r="B13" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24">
+      <c r="A14" s="23">
         <v>12</v>
       </c>
-      <c r="B14" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>23</v>
+      <c r="B14" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="17" t="s">
-        <v>39</v>
+      <c r="E14" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -1045,11 +1053,11 @@
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>34</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1059,11 +1067,11 @@
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="29" t="s">
         <v>34</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1073,15 +1081,15 @@
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="16" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="F17" s="4"/>
     </row>
@@ -1089,15 +1097,15 @@
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>23</v>
+      <c r="B18" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="17" t="s">
-        <v>39</v>
+      <c r="E18" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="F18" s="4"/>
     </row>
@@ -2189,7 +2197,7 @@
   <dimension ref="A1:F997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2203,70 +2211,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="C4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -10217,10 +10237,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
-  <dimension ref="A1:F997"/>
+  <dimension ref="A1:F996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10235,164 +10255,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="31"/>
+      <c r="A1" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="37"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="19" t="s">
+      <c r="E3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="50" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
         <v>10</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="17" t="s">
+      <c r="B5" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="30">
+        <v>12</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>16</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="30">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>12</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="30">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="50" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
-        <v>10</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="35">
-        <v>12</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
-        <v>16</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="35">
-        <v>8</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
-        <v>12</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="35">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="D8" s="38">
+        <v>3</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -10400,7 +10420,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -10425,16 +10445,9 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-    </row>
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="12.5" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:6" ht="12.5" x14ac:dyDescent="0.25"/>
     <row r="17" ht="12.5" x14ac:dyDescent="0.25"/>
     <row r="18" ht="12.5" x14ac:dyDescent="0.25"/>
@@ -11416,7 +11429,6 @@
     <row r="994" ht="12.5" x14ac:dyDescent="0.25"/>
     <row r="995" ht="12.5" x14ac:dyDescent="0.25"/>
     <row r="996" ht="12.5" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>